<commit_message>
scraper page display and fcc scrping
</commit_message>
<xml_diff>
--- a/sources/FCC_MAP_FINAL_FORMATTED.xlsx
+++ b/sources/FCC_MAP_FINAL_FORMATTED.xlsx
@@ -5,7 +5,7 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lotzconr\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Dev\lab\fcc.scraper\sources\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -1646,8 +1646,8 @@
   <sheetData>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="C2" s="1" t="str">
-        <f>"[    {"</f>
-        <v>[    {</v>
+        <f>" [{"</f>
+        <v xml:space="preserve"> [{</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
@@ -2283,8 +2283,8 @@
         <v>6</v>
       </c>
       <c r="C72" s="1" t="str">
-        <f>"""subheader"":{""name"":"""&amp;B72&amp;""","</f>
-        <v>"subheader":{"name":"Responsive Design with Bootstrap",</v>
+        <f>"""name"":"""&amp;B72&amp;""","</f>
+        <v>"name":"Responsive Design with Bootstrap",</v>
       </c>
     </row>
     <row r="73" spans="1:3" x14ac:dyDescent="0.25">
@@ -2572,8 +2572,8 @@
         <v>151</v>
       </c>
       <c r="C104" s="2" t="str">
-        <f>""""&amp;B104&amp;"""] } } , {"</f>
-        <v>"Use Comments to Clarify Code"] } } , {</v>
+        <f>""""&amp;B104&amp;"""]  } , {"</f>
+        <v>"Use Comments to Clarify Code"]  } , {</v>
       </c>
     </row>
     <row r="105" spans="1:3" x14ac:dyDescent="0.25">
@@ -2582,8 +2582,8 @@
         <v>7</v>
       </c>
       <c r="C105" s="1" t="str">
-        <f>"""subheader"":{""name"":"""&amp;B105&amp;""","</f>
-        <v>"subheader":{"name":"Gear up for Success",</v>
+        <f>"""name"":"""&amp;B105&amp;""","</f>
+        <v>"name":"Gear up for Success",</v>
       </c>
     </row>
     <row r="106" spans="1:3" x14ac:dyDescent="0.25">
@@ -2628,8 +2628,8 @@
         <v>343</v>
       </c>
       <c r="C110" s="2" t="str">
-        <f>""""&amp;B110&amp;"""] } } , {"</f>
-        <v>"Become a Supporter"] } } , {</v>
+        <f>""""&amp;B110&amp;"""]  } , {"</f>
+        <v>"Become a Supporter"]  } , {</v>
       </c>
     </row>
     <row r="111" spans="1:3" x14ac:dyDescent="0.25">
@@ -2638,8 +2638,8 @@
         <v>9</v>
       </c>
       <c r="C111" s="1" t="str">
-        <f>"""subheader"":{""name"":"""&amp;B111&amp;""","</f>
-        <v>"subheader":{"name":"jQuery",</v>
+        <f>"""name"":"""&amp;B111&amp;""","</f>
+        <v>"name":"jQuery",</v>
       </c>
     </row>
     <row r="112" spans="1:3" x14ac:dyDescent="0.25">
@@ -2810,8 +2810,8 @@
         <v>172</v>
       </c>
       <c r="C130" s="2" t="str">
-        <f>""""&amp;B130&amp;"""] } } , {"</f>
-        <v>"Use jQuery to Modify the Entire Page"] } } , {</v>
+        <f>""""&amp;B130&amp;"""]  } , {"</f>
+        <v>"Use jQuery to Modify the Entire Page"]  } , {</v>
       </c>
     </row>
     <row r="131" spans="1:3" x14ac:dyDescent="0.25">
@@ -2820,8 +2820,8 @@
         <v>11</v>
       </c>
       <c r="C131" s="1" t="str">
-        <f>"""subheader"":{""name"":"""&amp;B131&amp;""","</f>
-        <v>"subheader":{"name":"Basic Front End Development Projects",</v>
+        <f>"""name"":"""&amp;B131&amp;""","</f>
+        <v>"name":"Basic Front End Development Projects",</v>
       </c>
     </row>
     <row r="132" spans="1:3" x14ac:dyDescent="0.25">
@@ -2857,8 +2857,8 @@
         <v>175</v>
       </c>
       <c r="C135" s="2" t="str">
-        <f>""""&amp;B135&amp;"""] } } , {"</f>
-        <v>"Build a Personal Portfolio Webpage"] } } , {</v>
+        <f>""""&amp;B135&amp;"""]  } , {"</f>
+        <v>"Build a Personal Portfolio Webpage"]  } , {</v>
       </c>
     </row>
     <row r="136" spans="1:3" x14ac:dyDescent="0.25">
@@ -2867,8 +2867,8 @@
         <v>13</v>
       </c>
       <c r="C136" s="1" t="str">
-        <f>"""subheader"":{""name"":"""&amp;B136&amp;""","</f>
-        <v>"subheader":{"name":"Basic JavaScript",</v>
+        <f>"""name"":"""&amp;B136&amp;""","</f>
+        <v>"name":"Basic JavaScript",</v>
       </c>
     </row>
     <row r="137" spans="1:3" x14ac:dyDescent="0.25">
@@ -3813,8 +3813,8 @@
         <v>279</v>
       </c>
       <c r="C241" s="2" t="str">
-        <f>""""&amp;B241&amp;"""] } } , {"</f>
-        <v>"Invert Regular Expression Matches with JavaScript"] } } , {</v>
+        <f>""""&amp;B241&amp;"""]  } , {"</f>
+        <v>"Invert Regular Expression Matches with JavaScript"]  } , {</v>
       </c>
     </row>
     <row r="242" spans="1:3" x14ac:dyDescent="0.25">
@@ -3823,8 +3823,8 @@
         <v>15</v>
       </c>
       <c r="C242" s="1" t="str">
-        <f>"""subheader"":{""name"":"""&amp;B242&amp;""","</f>
-        <v>"subheader":{"name":"Object Oriented and Functional Programming",</v>
+        <f>"""name"":"""&amp;B242&amp;""","</f>
+        <v>"name":"Object Oriented and Functional Programming",</v>
       </c>
     </row>
     <row r="243" spans="1:3" x14ac:dyDescent="0.25">
@@ -3950,8 +3950,8 @@
         <v>292</v>
       </c>
       <c r="C256" s="2" t="str">
-        <f>""""&amp;B256&amp;"""] } } , {"</f>
-        <v>"Join Strings with .join"] } } , {</v>
+        <f>""""&amp;B256&amp;"""]  } , {"</f>
+        <v>"Join Strings with .join"]  } , {</v>
       </c>
     </row>
     <row r="257" spans="1:3" x14ac:dyDescent="0.25">
@@ -3960,8 +3960,8 @@
         <v>17</v>
       </c>
       <c r="C257" s="1" t="str">
-        <f>"""subheader"":{""name"":"""&amp;B257&amp;""","</f>
-        <v>"subheader":{"name":"Basic Algorithm Scripting",</v>
+        <f>"""name"":"""&amp;B257&amp;""","</f>
+        <v>"name":"Basic Algorithm Scripting",</v>
       </c>
     </row>
     <row r="258" spans="1:3" x14ac:dyDescent="0.25">
@@ -4123,8 +4123,8 @@
         <v>309</v>
       </c>
       <c r="C275" s="2" t="str">
-        <f>""""&amp;B275&amp;"""] } } , {"</f>
-        <v>"Caesars Cipher"] } } , {</v>
+        <f>""""&amp;B275&amp;"""]  } , {"</f>
+        <v>"Caesars Cipher"]  } , {</v>
       </c>
     </row>
     <row r="276" spans="1:3" x14ac:dyDescent="0.25">
@@ -4133,8 +4133,8 @@
         <v>18</v>
       </c>
       <c r="C276" s="1" t="str">
-        <f>"""subheader"":{""name"":"""&amp;B276&amp;""","</f>
-        <v>"subheader":{"name":"JSON APIs and Ajax",</v>
+        <f>"""name"":"""&amp;B276&amp;""","</f>
+        <v>"name":"JSON APIs and Ajax",</v>
       </c>
     </row>
     <row r="277" spans="1:3" x14ac:dyDescent="0.25">
@@ -4206,8 +4206,8 @@
         <v>316</v>
       </c>
       <c r="C284" s="2" t="str">
-        <f>""""&amp;B284&amp;"""] } } , {"</f>
-        <v>"Get Geo-location Data"] } } , {</v>
+        <f>""""&amp;B284&amp;"""]  } , {"</f>
+        <v>"Get Geo-location Data"]  } , {</v>
       </c>
     </row>
     <row r="285" spans="1:3" x14ac:dyDescent="0.25">
@@ -4216,8 +4216,8 @@
         <v>19</v>
       </c>
       <c r="C285" s="1" t="str">
-        <f>"""subheader"":{""name"":"""&amp;B285&amp;""","</f>
-        <v>"subheader":{"name":"Intermediate Front End Development Projects",</v>
+        <f>"""name"":"""&amp;B285&amp;""","</f>
+        <v>"name":"Intermediate Front End Development Projects",</v>
       </c>
     </row>
     <row r="286" spans="1:3" x14ac:dyDescent="0.25">
@@ -4262,8 +4262,8 @@
         <v>320</v>
       </c>
       <c r="C290" s="2" t="str">
-        <f>""""&amp;B290&amp;"""] } } , {"</f>
-        <v>"Use the Twitch.tv JSON API"] } } , {</v>
+        <f>""""&amp;B290&amp;"""]  } , {"</f>
+        <v>"Use the Twitch.tv JSON API"]  } , {</v>
       </c>
     </row>
     <row r="291" spans="1:3" x14ac:dyDescent="0.25">
@@ -4272,8 +4272,8 @@
         <v>21</v>
       </c>
       <c r="C291" s="1" t="str">
-        <f>"""subheader"":{""name"":"""&amp;B291&amp;""","</f>
-        <v>"subheader":{"name":"Intermediate Algorithm Scripting",</v>
+        <f>"""name"":"""&amp;B291&amp;""","</f>
+        <v>"name":"Intermediate Algorithm Scripting",</v>
       </c>
     </row>
     <row r="292" spans="1:3" x14ac:dyDescent="0.25">
@@ -4471,8 +4471,8 @@
         <v>393</v>
       </c>
       <c r="C313" s="2" t="str">
-        <f>""""&amp;B313&amp;"""] } } , {"</f>
-        <v>"Arguments Optional"] } } , {</v>
+        <f>""""&amp;B313&amp;"""]  } , {"</f>
+        <v>"Arguments Optional"]  } , {</v>
       </c>
     </row>
     <row r="314" spans="1:3" x14ac:dyDescent="0.25">
@@ -4481,8 +4481,8 @@
         <v>22</v>
       </c>
       <c r="C314" s="1" t="str">
-        <f>"""subheader"":{""name"":"""&amp;B314&amp;""","</f>
-        <v>"subheader":{"name":"Advanced Algorithm Scripting",</v>
+        <f>"""name"":"""&amp;B314&amp;""","</f>
+        <v>"name":"Advanced Algorithm Scripting",</v>
       </c>
     </row>
     <row r="315" spans="1:3" x14ac:dyDescent="0.25">
@@ -4572,8 +4572,8 @@
         <v>349</v>
       </c>
       <c r="C324" s="2" t="str">
-        <f>""""&amp;B324&amp;"""] } } , {"</f>
-        <v>"Pairwise"] } } , {</v>
+        <f>""""&amp;B324&amp;"""]  } , {"</f>
+        <v>"Pairwise"]  } , {</v>
       </c>
     </row>
     <row r="325" spans="1:3" x14ac:dyDescent="0.25">
@@ -4582,8 +4582,8 @@
         <v>23</v>
       </c>
       <c r="C325" s="1" t="str">
-        <f>"""subheader"":{""name"":"""&amp;B325&amp;""","</f>
-        <v>"subheader":{"name":"Advanced Front End Development Projects",</v>
+        <f>"""name"":"""&amp;B325&amp;""","</f>
+        <v>"name":"Advanced Front End Development Projects",</v>
       </c>
     </row>
     <row r="326" spans="1:3" x14ac:dyDescent="0.25">
@@ -4628,8 +4628,8 @@
         <v>352</v>
       </c>
       <c r="C330" s="2" t="str">
-        <f>""""&amp;B330&amp;"""] } } , {"</f>
-        <v>"Build a Simon Game"] } } , {</v>
+        <f>""""&amp;B330&amp;"""]  } , {"</f>
+        <v>"Build a Simon Game"]  } , {</v>
       </c>
     </row>
     <row r="331" spans="1:3" x14ac:dyDescent="0.25">
@@ -4638,8 +4638,8 @@
         <v>25</v>
       </c>
       <c r="C331" s="1" t="str">
-        <f>"""subheader"":{""name"":"""&amp;B331&amp;""","</f>
-        <v>"subheader":{"name":"Claim Your Front End Development Certificate",</v>
+        <f>"""name"":"""&amp;B331&amp;""","</f>
+        <v>"name":"Claim Your Front End Development Certificate",</v>
       </c>
     </row>
     <row r="332" spans="1:3" x14ac:dyDescent="0.25">
@@ -4657,8 +4657,8 @@
         <v>25</v>
       </c>
       <c r="C333" s="2" t="str">
-        <f>""""&amp;B333&amp;"""] } } ]  }, {"</f>
-        <v>"Claim Your Front End Development Certificate"] } } ]  }, {</v>
+        <f>""""&amp;B333&amp;"""] }  ]}  , {"</f>
+        <v>"Claim Your Front End Development Certificate"] }  ]}  , {</v>
       </c>
     </row>
     <row r="334" spans="1:3" x14ac:dyDescent="0.25">
@@ -4696,8 +4696,8 @@
         <v>353</v>
       </c>
       <c r="C337" s="2" t="str">
-        <f>""""&amp;B337&amp;"""] }  , {"</f>
-        <v>"Learn Sass Challenges"] }  , {</v>
+        <f>""""&amp;B337&amp;"""]  } , {"</f>
+        <v>"Learn Sass Challenges"]  } , {</v>
       </c>
     </row>
     <row r="338" spans="1:3" x14ac:dyDescent="0.25">
@@ -4706,8 +4706,8 @@
         <v>29</v>
       </c>
       <c r="C338" s="1" t="str">
-        <f>"""subheader"":{""name"":"""&amp;B338&amp;""","</f>
-        <v>"subheader":{"name":"React",</v>
+        <f>"""name"":"""&amp;B338&amp;""","</f>
+        <v>"name":"React",</v>
       </c>
     </row>
     <row r="339" spans="1:3" x14ac:dyDescent="0.25">
@@ -4725,8 +4725,8 @@
         <v>354</v>
       </c>
       <c r="C340" s="2" t="str">
-        <f>""""&amp;B340&amp;"""] } } , {"</f>
-        <v>"Learn React Challenges"] } } , {</v>
+        <f>""""&amp;B340&amp;"""]  } , {"</f>
+        <v>"Learn React Challenges"]  } , {</v>
       </c>
     </row>
     <row r="341" spans="1:3" x14ac:dyDescent="0.25">
@@ -4735,8 +4735,8 @@
         <v>30</v>
       </c>
       <c r="C341" s="1" t="str">
-        <f>"""subheader"":{""name"":"""&amp;B341&amp;""","</f>
-        <v>"subheader":{"name":"React Projects",</v>
+        <f>"""name"":"""&amp;B341&amp;""","</f>
+        <v>"name":"React Projects",</v>
       </c>
     </row>
     <row r="342" spans="1:3" x14ac:dyDescent="0.25">
@@ -4790,8 +4790,8 @@
         <v>359</v>
       </c>
       <c r="C347" s="2" t="str">
-        <f>""""&amp;B347&amp;"""] } } , {"</f>
-        <v>"Build a Roguelike Dungeon Crawler Game"] } } , {</v>
+        <f>""""&amp;B347&amp;"""]  } , {"</f>
+        <v>"Build a Roguelike Dungeon Crawler Game"]  } , {</v>
       </c>
     </row>
     <row r="348" spans="1:3" x14ac:dyDescent="0.25">
@@ -4800,8 +4800,8 @@
         <v>32</v>
       </c>
       <c r="C348" s="1" t="str">
-        <f>"""subheader"":{""name"":"""&amp;B348&amp;""","</f>
-        <v>"subheader":{"name":"D3",</v>
+        <f>"""name"":"""&amp;B348&amp;""","</f>
+        <v>"name":"D3",</v>
       </c>
     </row>
     <row r="349" spans="1:3" x14ac:dyDescent="0.25">
@@ -4819,8 +4819,8 @@
         <v>360</v>
       </c>
       <c r="C350" s="2" t="str">
-        <f>""""&amp;B350&amp;"""] } } , {"</f>
-        <v>"Learn D3 Challenges"] } } , {</v>
+        <f>""""&amp;B350&amp;"""]  } , {"</f>
+        <v>"Learn D3 Challenges"]  } , {</v>
       </c>
     </row>
     <row r="351" spans="1:3" x14ac:dyDescent="0.25">
@@ -4829,8 +4829,8 @@
         <v>33</v>
       </c>
       <c r="C351" s="1" t="str">
-        <f>"""subheader"":{""name"":"""&amp;B351&amp;""","</f>
-        <v>"subheader":{"name":"Data Visualization Projects",</v>
+        <f>"""name"":"""&amp;B351&amp;""","</f>
+        <v>"name":"Data Visualization Projects",</v>
       </c>
     </row>
     <row r="352" spans="1:3" x14ac:dyDescent="0.25">
@@ -4884,8 +4884,8 @@
         <v>365</v>
       </c>
       <c r="C357" s="2" t="str">
-        <f>""""&amp;B357&amp;"""] } } , {"</f>
-        <v>"Map Data Across the Globe"] } } , {</v>
+        <f>""""&amp;B357&amp;"""]  } , {"</f>
+        <v>"Map Data Across the Globe"]  } , {</v>
       </c>
     </row>
     <row r="358" spans="1:3" x14ac:dyDescent="0.25">
@@ -4894,8 +4894,8 @@
         <v>34</v>
       </c>
       <c r="C358" s="1" t="str">
-        <f>"""subheader"":{""name"":"""&amp;B358&amp;""","</f>
-        <v>"subheader":{"name":"Claim Your Data Visualization Certificate",</v>
+        <f>"""name"":"""&amp;B358&amp;""","</f>
+        <v>"name":"Claim Your Data Visualization Certificate",</v>
       </c>
     </row>
     <row r="359" spans="1:3" x14ac:dyDescent="0.25">
@@ -4913,8 +4913,8 @@
         <v>34</v>
       </c>
       <c r="C360" s="2" t="str">
-        <f>""""&amp;B360&amp;"""] } } ]  }, {"</f>
-        <v>"Claim Your Data Visualization Certificate"] } } ]  }, {</v>
+        <f>""""&amp;B360&amp;"""] }  ]}  , {"</f>
+        <v>"Claim Your Data Visualization Certificate"] }  ]}  , {</v>
       </c>
     </row>
     <row r="361" spans="1:3" x14ac:dyDescent="0.25">
@@ -4961,8 +4961,8 @@
         <v>367</v>
       </c>
       <c r="C365" s="2" t="str">
-        <f>""""&amp;B365&amp;"""] }  , {"</f>
-        <v>"Using typeof"] }  , {</v>
+        <f>""""&amp;B365&amp;"""]  } , {"</f>
+        <v>"Using typeof"]  } , {</v>
       </c>
     </row>
     <row r="366" spans="1:3" x14ac:dyDescent="0.25">
@@ -4971,8 +4971,8 @@
         <v>37</v>
       </c>
       <c r="C366" s="1" t="str">
-        <f>"""subheader"":{""name"":"""&amp;B366&amp;""","</f>
-        <v>"subheader":{"name":"Git",</v>
+        <f>"""name"":"""&amp;B366&amp;""","</f>
+        <v>"name":"Git",</v>
       </c>
     </row>
     <row r="367" spans="1:3" x14ac:dyDescent="0.25">
@@ -4990,8 +4990,8 @@
         <v>368</v>
       </c>
       <c r="C368" s="2" t="str">
-        <f>""""&amp;B368&amp;"""] } } , {"</f>
-        <v>"Save your Code Revisions Forever with Git"] } } , {</v>
+        <f>""""&amp;B368&amp;"""]  } , {"</f>
+        <v>"Save your Code Revisions Forever with Git"]  } , {</v>
       </c>
     </row>
     <row r="369" spans="1:3" x14ac:dyDescent="0.25">
@@ -5000,8 +5000,8 @@
         <v>38</v>
       </c>
       <c r="C369" s="1" t="str">
-        <f>"""subheader"":{""name"":"""&amp;B369&amp;""","</f>
-        <v>"subheader":{"name":"Node.js and Express.js",</v>
+        <f>"""name"":"""&amp;B369&amp;""","</f>
+        <v>"name":"Node.js and Express.js",</v>
       </c>
     </row>
     <row r="370" spans="1:3" x14ac:dyDescent="0.25">
@@ -5055,8 +5055,8 @@
         <v>373</v>
       </c>
       <c r="C375" s="2" t="str">
-        <f>""""&amp;B375&amp;"""] } } , {"</f>
-        <v>"Build Web Apps with Express.js"] } } , {</v>
+        <f>""""&amp;B375&amp;"""]  } , {"</f>
+        <v>"Build Web Apps with Express.js"]  } , {</v>
       </c>
     </row>
     <row r="376" spans="1:3" x14ac:dyDescent="0.25">
@@ -5065,8 +5065,8 @@
         <v>40</v>
       </c>
       <c r="C376" s="1" t="str">
-        <f>"""subheader"":{""name"":"""&amp;B376&amp;""","</f>
-        <v>"subheader":{"name":"MongoDB",</v>
+        <f>"""name"":"""&amp;B376&amp;""","</f>
+        <v>"name":"MongoDB",</v>
       </c>
     </row>
     <row r="377" spans="1:3" x14ac:dyDescent="0.25">
@@ -5084,8 +5084,8 @@
         <v>374</v>
       </c>
       <c r="C378" s="2" t="str">
-        <f>""""&amp;B378&amp;"""] } } , {"</f>
-        <v>"Store Data in MongoDB"] } } , {</v>
+        <f>""""&amp;B378&amp;"""]  } , {"</f>
+        <v>"Store Data in MongoDB"]  } , {</v>
       </c>
     </row>
     <row r="379" spans="1:3" x14ac:dyDescent="0.25">
@@ -5094,8 +5094,8 @@
         <v>41</v>
       </c>
       <c r="C379" s="1" t="str">
-        <f>"""subheader"":{""name"":"""&amp;B379&amp;""","</f>
-        <v>"subheader":{"name":"API Projects",</v>
+        <f>"""name"":"""&amp;B379&amp;""","</f>
+        <v>"name":"API Projects",</v>
       </c>
     </row>
     <row r="380" spans="1:3" x14ac:dyDescent="0.25">
@@ -5158,8 +5158,8 @@
         <v>380</v>
       </c>
       <c r="C386" s="2" t="str">
-        <f>""""&amp;B386&amp;"""] } } , {"</f>
-        <v>"File Metadata Microservice"] } } , {</v>
+        <f>""""&amp;B386&amp;"""]  } , {"</f>
+        <v>"File Metadata Microservice"]  } , {</v>
       </c>
     </row>
     <row r="387" spans="1:3" x14ac:dyDescent="0.25">
@@ -5168,8 +5168,8 @@
         <v>42</v>
       </c>
       <c r="C387" s="1" t="str">
-        <f>"""subheader"":{""name"":"""&amp;B387&amp;""","</f>
-        <v>"subheader":{"name":"Dynamic Web Application Projects",</v>
+        <f>"""name"":"""&amp;B387&amp;""","</f>
+        <v>"name":"Dynamic Web Application Projects",</v>
       </c>
     </row>
     <row r="388" spans="1:3" x14ac:dyDescent="0.25">
@@ -5232,8 +5232,8 @@
         <v>386</v>
       </c>
       <c r="C394" s="2" t="str">
-        <f>""""&amp;B394&amp;"""] } } , {"</f>
-        <v>"Build a Pinterest Clone"] } } , {</v>
+        <f>""""&amp;B394&amp;"""]  } , {"</f>
+        <v>"Build a Pinterest Clone"]  } , {</v>
       </c>
     </row>
     <row r="395" spans="1:3" x14ac:dyDescent="0.25">
@@ -5242,8 +5242,8 @@
         <v>44</v>
       </c>
       <c r="C395" s="1" t="str">
-        <f>"""subheader"":{""name"":"""&amp;B395&amp;""","</f>
-        <v>"subheader":{"name":"Claim Your Back End Development Certificate",</v>
+        <f>"""name"":"""&amp;B395&amp;""","</f>
+        <v>"name":"Claim Your Back End Development Certificate",</v>
       </c>
     </row>
     <row r="396" spans="1:3" x14ac:dyDescent="0.25">
@@ -5261,8 +5261,8 @@
         <v>44</v>
       </c>
       <c r="C397" s="2" t="str">
-        <f>""""&amp;B397&amp;"""]  } ]  }, {"</f>
-        <v>"Claim Your Back End Development Certificate"]  } ]  }, {</v>
+        <f>""""&amp;B397&amp;"""] }  ]}  , {"</f>
+        <v>"Claim Your Back End Development Certificate"] }  ]}  , {</v>
       </c>
     </row>
     <row r="398" spans="1:3" x14ac:dyDescent="0.25">
@@ -5336,8 +5336,8 @@
         <v>46</v>
       </c>
       <c r="C405" s="2" t="str">
-        <f>""""&amp;B405&amp;"""] } } ]  }, {"</f>
-        <v>"Claim your Full Stack Development Certification"] } } ]  }, {</v>
+        <f>""""&amp;B405&amp;"""] }  ]}  , {"</f>
+        <v>"Claim your Full Stack Development Certification"] }  ]}  , {</v>
       </c>
     </row>
     <row r="406" spans="1:3" x14ac:dyDescent="0.25">
@@ -5393,8 +5393,8 @@
         <v>50</v>
       </c>
       <c r="C411" s="2" t="str">
-        <f>""""&amp;B411&amp;"""] }  , {"</f>
-        <v>"Whiteboard Coding Training"] }  , {</v>
+        <f>""""&amp;B411&amp;"""]  } , {"</f>
+        <v>"Whiteboard Coding Training"]  } , {</v>
       </c>
     </row>
     <row r="412" spans="1:3" x14ac:dyDescent="0.25">
@@ -5403,8 +5403,8 @@
         <v>388</v>
       </c>
       <c r="C412" s="1" t="str">
-        <f>"""subheader"":{""name"":"""&amp;B412&amp;""","</f>
-        <v>"subheader":{"name":"Mock Interviews",</v>
+        <f>"""name"":"""&amp;B412&amp;""","</f>
+        <v>"name":"Mock Interviews",</v>
       </c>
     </row>
     <row r="413" spans="1:3" x14ac:dyDescent="0.25">

</xml_diff>